<commit_message>
Updated Excel spreadhseet with latest results
</commit_message>
<xml_diff>
--- a/performance/picar_peformance_benchmark.xlsx
+++ b/performance/picar_peformance_benchmark.xlsx
@@ -80,14 +80,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="0.000000"/>
   </numFmts>
   <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -109,17 +111,20 @@
       <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="12"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -178,7 +183,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -189,6 +194,10 @@
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -223,14 +232,14 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3:F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="52.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="26.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="26.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="21.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="22.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="22.92"/>
@@ -266,18 +275,18 @@
       <c r="C2" s="3" t="n">
         <v>0.00148004899999421</v>
       </c>
-      <c r="D2" s="3" t="n">
+      <c r="D2" s="4" t="n">
         <v>18.311</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="3" t="n">
+      <c r="F2" s="4" t="n">
         <v>1447</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="6" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="3" t="n">
@@ -286,13 +295,13 @@
       <c r="C3" s="3" t="n">
         <v>0.00148004899999421</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="4" t="s">
         <v>10</v>
       </c>
     </row>
@@ -306,13 +315,13 @@
       <c r="C4" s="3" t="n">
         <v>0.00189432999997052</v>
       </c>
-      <c r="D4" s="3" t="n">
+      <c r="D4" s="4" t="n">
         <v>18.993</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="3" t="n">
+      <c r="F4" s="4" t="n">
         <v>1363</v>
       </c>
     </row>
@@ -326,13 +335,13 @@
       <c r="C5" s="3" t="n">
         <v>0.00189432999997052</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="4" t="s">
         <v>10</v>
       </c>
     </row>
@@ -346,13 +355,13 @@
       <c r="C6" s="3" t="n">
         <v>0.0122609919999945</v>
       </c>
-      <c r="D6" s="3" t="n">
+      <c r="D6" s="4" t="n">
         <v>23.289</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F6" s="3" t="n">
+      <c r="F6" s="4" t="n">
         <v>1441</v>
       </c>
     </row>
@@ -366,13 +375,13 @@
       <c r="C7" s="3" t="n">
         <v>0.0122609919999945</v>
       </c>
-      <c r="D7" s="3" t="n">
+      <c r="D7" s="4" t="n">
         <v>28.022</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F7" s="3" t="n">
+      <c r="F7" s="4" t="n">
         <v>1295</v>
       </c>
     </row>

</xml_diff>